<commit_message>
updated MC + plotting with boxplots
</commit_message>
<xml_diff>
--- a/examples/puerto_rico/data/data.xlsx
+++ b/examples/puerto_rico/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="941" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="941" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -1305,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1615,7 @@
         <v>132</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>131</v>
@@ -1641,7 +1641,7 @@
         <v>132</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>131</v>
@@ -1771,7 +1771,7 @@
         <v>131</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>132</v>
@@ -1797,7 +1797,7 @@
         <v>131</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>132</v>
@@ -1927,7 +1927,7 @@
         <v>131</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>132</v>
@@ -1953,7 +1953,7 @@
         <v>131</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>132</v>
@@ -6419,7 +6419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>

</xml_diff>